<commit_message>
Practice 01 - Solution
</commit_message>
<xml_diff>
--- a/me/2.Asynchronous-ProgrammingChương-Asynchronous-Programming/6.Bai-tap-thuc-hanh-so-01-02.xlsx
+++ b/me/2.Asynchronous-ProgrammingChương-Asynchronous-Programming/6.Bai-tap-thuc-hanh-so-01-02.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/javascript_advance/me/2.Asynchronous-ProgrammingChương-Asynchronous-Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D0569E-7CD8-674A-B269-6F8838555354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F014DB9B-EA97-CD43-B79E-14AA586C3FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="1740" windowWidth="31740" windowHeight="18760" xr2:uid="{7676CE1B-4587-7A49-84A8-63238B5A3602}"/>
+    <workbookView xWindow="2240" yWindow="1740" windowWidth="31740" windowHeight="18760" activeTab="1" xr2:uid="{7676CE1B-4587-7A49-84A8-63238B5A3602}"/>
   </bookViews>
   <sheets>
     <sheet name="Practice 01" sheetId="1" r:id="rId1"/>
+    <sheet name="Practice 01 - Solution" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="84">
   <si>
     <t>構成</t>
   </si>
@@ -309,6 +310,219 @@
       <t xml:space="preserve"> cho nên mình sẽ không biết dữ liệu nào là dữ liệu được hoàn thành trước, dữ liệu nào là dữ liệu được hoàn thành sau</t>
     </r>
   </si>
+  <si>
+    <t>Giải quyết bài toán đó là gọi API theo đúng thứ tự, tiếp cận vấn đề 1 cách đơn giản nhất trước khi đi sâu vào JS liên quan đến vấn đề xử lý bất đồng bộ</t>
+  </si>
+  <si>
+    <t>solution_01.js</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;!DOCTYPE html&gt;
+&lt;html lang="en"&gt;
+&lt;head&gt;
+  &lt;meta charset="UTF-8"&gt;
+  &lt;meta http-equiv="X-UA-Compatible" content="IE=edge"&gt;
+  &lt;meta name="viewport" content="width=device-width, initial-scale=1.0"&gt;
+  &lt;title&gt;Challenge Async 01&lt;/title&gt;
+&lt;/head&gt;
+&lt;body&gt;
+  &lt;h1&gt;Challenge 01 - Async Basic&lt;/h1&gt;
+&lt;/body&gt;
+&lt;!-- &lt;script src="challenge_01.js"&gt;&lt;/script&gt; --&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>&lt;script src="solution_01.js"&gt;&lt;/script&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&lt;!-- &lt;script src="challenge_02.js"&gt;&lt;/script&gt; --&gt;
+&lt;!-- &lt;script src="solution_02.js"&gt;&lt;/script&gt; --&gt;
+&lt;/html&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>javascript_advance/02_async_programming/04_Bai-tap-thuc-hanh-so-01-02/solution_01.js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  var fakeResponses = {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "https://quangvu.com/api/1": "Data1",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "https://quangvu.com/api/2": "Data2",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "https://quangvu.com/api/3": "Data3"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  };</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  var randomMiliseconds = Math.floor(Math.random() * 5000) + 1000;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  console.log(`Đang gọi API với URL : ${url} - Thời gian ${randomMiliseconds}ms`);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  setTimeout(function(){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    callbackFn(fakeResponses[url]);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  }, randomMiliseconds);</t>
+  </si>
+  <si>
+    <t>/**</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * Yêu cầu Challenge 01:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> *  1. Các lời gọi API sẽ có thời gian chạy khác nhau và ngâu nhiên</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> *  2. Kết quả phải được hiển thị ra cho người dùng theo đúng thứ tự 1 -&gt; 2 -&gt; 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> */</t>
+  </si>
+  <si>
+    <t>fakeGetData('https://quangvu.com/api/1', function(res1) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  fakeGetData('https://quangvu.com/api/2', function(res2) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    fakeGetData('https://quangvu.com/api/3', function(res3) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      console.log(res1);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      console.log(res2);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      console.log(res3);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    })</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  })</t>
+  </si>
+  <si>
+    <t>})</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Giả lập khi setTimeout xong thì sẽ gọi lại hàm call back callbackFn và hàm callbackFn này sẽ truyền cho mình dữ liệu, có nghĩa là khi </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>tham số thứ 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> được gọi là lúc API được gọi xong</t>
+    </r>
+  </si>
+  <si>
+    <t>Gọi API thứ nhất</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gọi API thứ 2 </t>
+  </si>
+  <si>
+    <t>Check by browser</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gọi API thứ 3. Mình đã nắm được các vấn đề liên quan đến Higher Order Function và cái quan trọng nhất là Closure liên quan đến Scope trong Javascript, cho nên function con ở bên trong này có có thể truy cập được vào </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>các biến ở bên ngoài</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(res1 và res2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mình đang tiếp cận theo hướng đầu tiên đó là gọi lần lượt từng API một, hướng tiếp cận này nếu áp dụng vào thực tế thì sẽ không tốt vì lúc đó thời gian chạy là </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>thời gian tổng của cả 3 API</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, thay vào đó mình cần tìm 1 kỹ thuật nào đó để có thể gọi </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">song song, lúc đó </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>thời gian chạy sẽ là thời gian của API lâu nhất</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -340,12 +554,18 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -440,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -451,8 +671,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -465,7 +686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -480,9 +701,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,6 +827,373 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AB51674-E376-63FF-D806-05B1811251DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3060700" y="14795500"/>
+          <a:ext cx="12700000" cy="2146300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41A051D1-BCC9-6956-0E1F-36E506902B07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1168400" y="14808200"/>
+          <a:ext cx="1625600" cy="2133600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{152E122D-7265-D41D-F457-72E59A2EB895}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1168400" y="17043400"/>
+          <a:ext cx="2527300" cy="1727200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1C639C8-20B8-346C-2E13-EE75D6929E08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2489200" y="17030700"/>
+          <a:ext cx="1739900" cy="1752600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E953D89-3735-C11B-7D97-70DBA6889385}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2159000" y="19278600"/>
+          <a:ext cx="20345400" cy="139700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55A95EBD-F753-2786-0560-E5F8923410FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2184400" y="19291300"/>
+          <a:ext cx="20866100" cy="368300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>97564</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBB024C1-FF8B-9BA4-99B1-57298E1799A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="939800" y="21805900"/>
+          <a:ext cx="15240000" cy="3894864"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -910,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E5BE13-EF95-2744-874B-F0991DD5CCB3}">
   <dimension ref="A4:K85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="M87" sqref="M87"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1178,14 +1766,14 @@
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
-      <c r="E41" s="10" t="s">
+      <c r="E41" t="s">
         <v>5</v>
       </c>
       <c r="G41" s="5"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" s="4"/>
-      <c r="E42" s="10" t="s">
+      <c r="E42" t="s">
         <v>7</v>
       </c>
       <c r="G42" s="5"/>
@@ -1238,168 +1826,168 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="14"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="15"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="17"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="16"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="15"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="17"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="16"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B53" s="15"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="17"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="16"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B54" s="15"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="17"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="16"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="15"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="17"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="16"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="15"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="17"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="16"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="15"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="17"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="16"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B58" s="15"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="17"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="16"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B59" s="15"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="17"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="16"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B60" s="15"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="17"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="16"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B61" s="15"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="17"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="16"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="15"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="17"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="16"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="15"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="17"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="16"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="15"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="17"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="16"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B65" s="15"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="17"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="16"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B66" s="18"/>
-      <c r="C66" s="19"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="19"/>
-      <c r="H66" s="20"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="19"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B67" s="21"/>
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="21"/>
-      <c r="G67" s="21"/>
-      <c r="H67" s="21"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
@@ -1426,84 +2014,48 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B71" s="4"/>
-      <c r="C71" s="11" t="s">
+      <c r="C71" t="s">
         <v>30</v>
       </c>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
       <c r="I71" s="5"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B72" s="4"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="11"/>
       <c r="I72" s="5"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B73" s="4"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11" t="s">
+      <c r="D73" t="s">
         <v>31</v>
       </c>
-      <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
       <c r="I73" s="5"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B74" s="4"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11" t="s">
+      <c r="D74" t="s">
         <v>32</v>
       </c>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
       <c r="I74" s="5"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B75" s="4"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11" t="s">
+      <c r="D75" t="s">
         <v>33</v>
       </c>
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="11"/>
       <c r="I75" s="5"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B76" s="4"/>
-      <c r="C76" s="11" t="s">
+      <c r="C76" t="s">
         <v>34</v>
       </c>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B77" s="4"/>
-      <c r="C77" s="11" t="s">
+      <c r="C77" t="s">
         <v>35</v>
       </c>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
       <c r="I77" s="5"/>
       <c r="J77" t="s">
         <v>24</v>
@@ -1514,24 +2066,13 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B78" s="4"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11"/>
       <c r="I78" s="5"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B79" s="4"/>
-      <c r="C79" s="11" t="s">
+      <c r="C79" t="s">
         <v>36</v>
       </c>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
       <c r="I79" s="5"/>
       <c r="J79" t="s">
         <v>24</v>
@@ -1542,24 +2083,13 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B80" s="4"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
-      <c r="G80" s="11"/>
-      <c r="H80" s="11"/>
       <c r="I80" s="5"/>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B81" s="4"/>
-      <c r="C81" s="11" t="s">
+      <c r="C81" t="s">
         <v>37</v>
       </c>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="11"/>
-      <c r="H81" s="11"/>
       <c r="I81" s="5"/>
       <c r="J81" t="s">
         <v>24</v>
@@ -1570,26 +2100,16 @@
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B82" s="4"/>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11" t="s">
+      <c r="D82" t="s">
         <v>38</v>
       </c>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
       <c r="I82" s="5"/>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B83" s="4"/>
-      <c r="C83" s="11" t="s">
+      <c r="C83" t="s">
         <v>39</v>
       </c>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
-      <c r="G83" s="11"/>
-      <c r="H83" s="11"/>
       <c r="I83" s="5"/>
       <c r="J83" t="s">
         <v>24</v>
@@ -1602,12 +2122,6 @@
       <c r="B84" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="11"/>
-      <c r="F84" s="11"/>
-      <c r="G84" s="11"/>
-      <c r="H84" s="11"/>
       <c r="I84" s="5"/>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.2">
@@ -1627,4 +2141,877 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{292D482B-F9AF-3948-B1F7-66105A7C8BA8}">
+  <dimension ref="A3:J107"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="L101" sqref="L101"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="4"/>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="4"/>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="4"/>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="4"/>
+      <c r="D31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="4"/>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="4"/>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="4"/>
+      <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="4"/>
+      <c r="D36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="4"/>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="4"/>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="4"/>
+      <c r="D39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" s="4"/>
+      <c r="E40" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B41" s="4"/>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B42" s="4"/>
+      <c r="D42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" s="4"/>
+      <c r="E43" t="s">
+        <v>5</v>
+      </c>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="4"/>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="4"/>
+      <c r="D45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="9"/>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="4"/>
+      <c r="E46" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="4"/>
+      <c r="E47" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B48" s="4"/>
+      <c r="E48" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G48" s="5"/>
+      <c r="H48" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="8"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B53" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="13"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B54" s="14"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="16"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B55" s="14"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="16"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B56" s="14"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="16"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B57" s="14"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="16"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B58" s="14"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="16"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B59" s="14"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="16"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B60" s="14"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="16"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B61" s="14"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="16"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B62" s="14"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="16"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B63" s="14"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="16"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B64" s="14"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="16"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B65" s="14"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="16"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B66" s="14"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="16"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B67" s="14"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="16"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B68" s="14"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="16"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B69" s="17"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="19"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B73" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="3"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B74" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="5"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B75" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="21"/>
+      <c r="H75" s="5"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B76" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="21"/>
+      <c r="G76" s="21"/>
+      <c r="H76" s="5"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B77" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="21"/>
+      <c r="H77" s="5"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B78" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C78" s="21"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="21"/>
+      <c r="H78" s="5"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B79" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="21"/>
+      <c r="H79" s="5"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B80" s="4"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="21"/>
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B81" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="21"/>
+      <c r="G81" s="21"/>
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B82" s="4"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="21"/>
+      <c r="E82" s="21"/>
+      <c r="F82" s="21"/>
+      <c r="G82" s="21"/>
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B83" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C83" s="21"/>
+      <c r="D83" s="21"/>
+      <c r="E83" s="21"/>
+      <c r="F83" s="21"/>
+      <c r="G83" s="21"/>
+      <c r="H83" s="5"/>
+    </row>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B84" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="21"/>
+      <c r="F84" s="21"/>
+      <c r="G84" s="21"/>
+      <c r="H84" s="5"/>
+      <c r="I84" t="s">
+        <v>24</v>
+      </c>
+      <c r="J84" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B85" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="21"/>
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B86" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C86" s="21"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="21"/>
+      <c r="G86" s="21"/>
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B87" s="4"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="21"/>
+      <c r="E87" s="21"/>
+      <c r="F87" s="21"/>
+      <c r="G87" s="21"/>
+      <c r="H87" s="5"/>
+    </row>
+    <row r="88" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B88" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C88" s="21"/>
+      <c r="D88" s="21"/>
+      <c r="E88" s="21"/>
+      <c r="F88" s="21"/>
+      <c r="G88" s="21"/>
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B89" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C89" s="21"/>
+      <c r="D89" s="21"/>
+      <c r="E89" s="21"/>
+      <c r="F89" s="21"/>
+      <c r="G89" s="21"/>
+      <c r="H89" s="5"/>
+    </row>
+    <row r="90" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B90" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C90" s="21"/>
+      <c r="D90" s="21"/>
+      <c r="E90" s="21"/>
+      <c r="F90" s="21"/>
+      <c r="G90" s="21"/>
+      <c r="H90" s="5"/>
+    </row>
+    <row r="91" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B91" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C91" s="21"/>
+      <c r="D91" s="21"/>
+      <c r="E91" s="21"/>
+      <c r="F91" s="21"/>
+      <c r="G91" s="21"/>
+      <c r="H91" s="5"/>
+    </row>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B92" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C92" s="21"/>
+      <c r="D92" s="21"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="21"/>
+      <c r="G92" s="21"/>
+      <c r="H92" s="5"/>
+    </row>
+    <row r="93" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B93" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C93" s="21"/>
+      <c r="D93" s="21"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="21"/>
+      <c r="H93" s="5"/>
+      <c r="I93" t="s">
+        <v>24</v>
+      </c>
+      <c r="J93" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="94" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B94" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C94" s="21"/>
+      <c r="D94" s="21"/>
+      <c r="E94" s="21"/>
+      <c r="F94" s="21"/>
+      <c r="G94" s="21"/>
+      <c r="H94" s="5"/>
+      <c r="I94" t="s">
+        <v>24</v>
+      </c>
+      <c r="J94" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="95" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B95" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C95" s="21"/>
+      <c r="D95" s="21"/>
+      <c r="E95" s="21"/>
+      <c r="F95" s="21"/>
+      <c r="G95" s="21"/>
+      <c r="H95" s="5"/>
+      <c r="I95" t="s">
+        <v>24</v>
+      </c>
+      <c r="J95" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="96" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B96" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C96" s="21"/>
+      <c r="D96" s="21"/>
+      <c r="E96" s="21"/>
+      <c r="F96" s="21"/>
+      <c r="G96" s="21"/>
+      <c r="H96" s="5"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B97" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C97" s="21"/>
+      <c r="D97" s="21"/>
+      <c r="E97" s="21"/>
+      <c r="F97" s="21"/>
+      <c r="G97" s="21"/>
+      <c r="H97" s="5"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B98" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C98" s="21"/>
+      <c r="D98" s="21"/>
+      <c r="E98" s="21"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="21"/>
+      <c r="H98" s="5"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B99" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C99" s="21"/>
+      <c r="D99" s="21"/>
+      <c r="E99" s="21"/>
+      <c r="F99" s="21"/>
+      <c r="G99" s="21"/>
+      <c r="H99" s="5"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B100" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C100" s="21"/>
+      <c r="D100" s="21"/>
+      <c r="E100" s="21"/>
+      <c r="F100" s="21"/>
+      <c r="G100" s="21"/>
+      <c r="H100" s="5"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B101" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C101" s="21"/>
+      <c r="D101" s="21"/>
+      <c r="E101" s="21"/>
+      <c r="F101" s="21"/>
+      <c r="G101" s="21"/>
+      <c r="H101" s="5"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B102" s="6"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
+      <c r="F102" s="7"/>
+      <c r="G102" s="7"/>
+      <c r="H102" s="8"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B53:H69"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Practice 02 - Solution 01
</commit_message>
<xml_diff>
--- a/me/2.Asynchronous-ProgrammingChương-Asynchronous-Programming/6.Bai-tap-thuc-hanh-so-01-02.xlsx
+++ b/me/2.Asynchronous-ProgrammingChương-Asynchronous-Programming/6.Bai-tap-thuc-hanh-so-01-02.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/javascript_advance/me/2.Asynchronous-ProgrammingChương-Asynchronous-Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127C8624-B662-8B45-9A5F-E8654108EC28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242E6D0D-8397-6E4C-A512-8022BEA70271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="1740" windowWidth="31740" windowHeight="18760" activeTab="2" xr2:uid="{7676CE1B-4587-7A49-84A8-63238B5A3602}"/>
+    <workbookView xWindow="2240" yWindow="1740" windowWidth="31740" windowHeight="18760" activeTab="3" xr2:uid="{7676CE1B-4587-7A49-84A8-63238B5A3602}"/>
   </bookViews>
   <sheets>
     <sheet name="Practice 01" sheetId="1" r:id="rId1"/>
     <sheet name="Practice 01 - Solution" sheetId="2" r:id="rId2"/>
     <sheet name="Practice 02" sheetId="3" r:id="rId3"/>
+    <sheet name="Practice 02 - Solution 01" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="129">
   <si>
     <t>構成</t>
   </si>
@@ -568,6 +569,395 @@
   </si>
   <si>
     <t xml:space="preserve">nhưng mình cần lưu dữ liệu lại ở đâu đó để chờ API1 chạy xong thì cho in API1 rồi đến API2 rồi đến API3 </t>
+  </si>
+  <si>
+    <t>solution_02.js</t>
+  </si>
+  <si>
+    <t>javascript_advance/02_async_programming/04_Bai-tap-thuc-hanh-so-01-02/solution_02.js</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;!DOCTYPE html&gt;
+&lt;html lang="en"&gt;
+&lt;head&gt;
+  &lt;meta charset="UTF-8"&gt;
+  &lt;meta http-equiv="X-UA-Compatible" content="IE=edge"&gt;
+  &lt;meta name="viewport" content="width=device-width, initial-scale=1.0"&gt;
+  &lt;title&gt;Challenge Async 01&lt;/title&gt;
+&lt;/head&gt;
+&lt;body&gt;
+  &lt;h1&gt;Challenge 01 - Async Basic&lt;/h1&gt;
+&lt;/body&gt;
+&lt;!-- &lt;script src="challenge_01.js"&gt;&lt;/script&gt; --&gt;
+&lt;!-- &lt;script src="solution_01.js"&gt;&lt;/script&gt; --&gt;
+&lt;!-- &lt;script src="challenge_02.js"&gt;&lt;/script&gt; --&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>&lt;script src="solution_02.js"&gt;&lt;/script&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&lt;/html&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>// debugger;</t>
+  </si>
+  <si>
+    <t>// Design Pattern</t>
+  </si>
+  <si>
+    <t>function startRunAPI(url) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  let res = null;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  fakeGetData(url, function(data) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      res = data;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  return function getData(cbFn) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      cbFn(res);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  }</t>
+  </si>
+  <si>
+    <t>let fnGetData1 = startRunAPI('https://quangvu.com/api/1'); // thunk</t>
+  </si>
+  <si>
+    <t>let fnGetData2 = startRunAPI('https://quangvu.com/api/2'); // thunk</t>
+  </si>
+  <si>
+    <t>let fnGetData3 = startRunAPI('https://quangvu.com/api/3'); // thunk</t>
+  </si>
+  <si>
+    <t>fnGetData1(function(res1) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  console.log(res1)</t>
+  </si>
+  <si>
+    <t>Giả lập có lời gọi API</t>
+  </si>
+  <si>
+    <t>Áp dụng kỹ thuật liên quan đến Higher Order Function return về 1 function. Khi nào cần lấy thì mới gọi đến function này</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ví dụ như ở trường hợp này thì API2 và API3 trong 2s đầu tiên đã chạy xong rồi, tuy nhiên cần phải chờ API1 chạy xong thì mới được in ra dữ liệu, trong quá trình chờ thì phải </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>lưu kết quả</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lại</t>
+    </r>
+  </si>
+  <si>
+    <t>function để bắt đầu gọi API, bởi vì mình muốn cả 3 API được gọi đồng thời nên mình dùng hàm này để bắt đầu gọi API</t>
+  </si>
+  <si>
+    <t>Dùng để giả lập gọi API</t>
+  </si>
+  <si>
+    <t>Gọi hàm và mình truyền vào 1 function để nhận được data</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sở dĩ không gọi trực tiếp hàm fakeGetData() bởi vì mình cần phải </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">lưu trữ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">dữ liệu lại, khi nào cần lấy data thì </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>gọi hàm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do đó mình taọ thêm </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">hàm mới </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>để giới hạn tầm vực lại. Mỗi API có 1 Scope riêng để lưu dữ liệu riêng</t>
+    </r>
+  </si>
+  <si>
+    <t>Gọi hàm fakeGetData() xong có nghĩa là đã gọi API xong thì mình sẽ lưu data vào res</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mình có 2 Scope cùng cấp nên mình tạo thêm biến </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> này ở Scope to hơn để lưu lại data response trả về từ API và chia sẻ biến giữa 2 hàm(scope) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gọi hàm call back </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>cbFn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> để truyền ngược </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> về bên dưới</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">null. Đoạn này luôn luôn in ra giá trị là </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> bởi vì đoạn gọi hàm </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>fnGetData1()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> này luôn luôn được coi là đoạn code đồng bộ ở trong Javascript do đó đoạn này luôn luôn được gọi trước các lời gọi API(mà ở mô phỏng này đó </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">là </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">setTimeout() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">nên setTimeout() luôn luôn được gọi sau nên khi mình gọi </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>fnGetData1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> thì giá trị </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>res</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lúc đó vẫn đang là </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nên </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>res1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> luôn luôn là giá trị null</t>
+    </r>
+  </si>
+  <si>
+    <t>Check browser</t>
   </si>
 </sst>
 </file>
@@ -706,7 +1096,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -750,6 +1140,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1240,6 +1631,908 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90CC0AD3-EB92-D2A5-DA81-A887E8F1508D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1054100" y="14998700"/>
+          <a:ext cx="431800" cy="7239000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02A36A28-8789-6D6A-3A92-45DD47E9ECB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1701800" y="23977600"/>
+          <a:ext cx="406400" cy="1663700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5679BC4-D40E-4424-C80D-20390FD7D561}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1028700" y="25793700"/>
+          <a:ext cx="558800" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99169E7B-9522-94B5-8238-37DACBAAFECF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1790700" y="23926800"/>
+          <a:ext cx="889000" cy="2590800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C7EB024-3561-2C1E-3397-8253E0D9486E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12496800" y="20726400"/>
+          <a:ext cx="6921500" cy="3111500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B5FC44-18F8-1052-E597-5A5CEBD3270C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2247900" y="24003000"/>
+          <a:ext cx="12814300" cy="1676400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DDB7F7A-4A10-CCFC-73FD-4E0A4B0D0268}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1663700" y="21513800"/>
+          <a:ext cx="15316200" cy="4165600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CEBE2C1-87D7-B33E-286C-1DDC18ECFB93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1676400" y="21678900"/>
+          <a:ext cx="7302500" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A3D0290-C253-F487-541F-299D2EFC29BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2146300" y="21704300"/>
+          <a:ext cx="6858000" cy="2133600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Straight Arrow Connector 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56286E26-00AD-EFA2-2987-86163691FF94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1752600" y="20726400"/>
+          <a:ext cx="17640300" cy="3098800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Arrow Connector 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E59B019C-53D7-49ED-5F64-1DA48913AA9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2324100" y="23152100"/>
+          <a:ext cx="8547100" cy="1498600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>143007</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>250692</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>106304</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E7483FE-F8A2-C353-2CFD-1B7F30568A2E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="968507" y="26047700"/>
+          <a:ext cx="14966685" cy="3522604"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Straight Arrow Connector 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{236732C8-58EC-D8EB-7215-E5FBB6AC2A29}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1638300" y="22136100"/>
+          <a:ext cx="6845300" cy="2946400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="Straight Arrow Connector 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48873E03-FF0E-F7BA-84B3-097F164D02E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1244600" y="21729700"/>
+          <a:ext cx="13144500" cy="3340100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="Straight Arrow Connector 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7965282A-3B8F-BB4F-C52D-B1E99F1F21CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1231900" y="21755100"/>
+          <a:ext cx="292100" cy="1320800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Straight Arrow Connector 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED38046A-958C-8A29-7049-F5E380D0D400}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2413000" y="24777700"/>
+          <a:ext cx="13931900" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Straight Arrow Connector 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6C02960-0383-4EB4-92E6-1366CBF3941D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1257300" y="24968200"/>
+          <a:ext cx="495300" cy="4216400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2193,8 +3486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{292D482B-F9AF-3948-B1F7-66105A7C8BA8}">
   <dimension ref="A3:J107"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2926,8 +4219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171CB472-A502-FD4D-86EA-E8CFCD4D7345}">
   <dimension ref="A4:K81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L73" sqref="L73"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3236,14 +4529,14 @@
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" s="4"/>
-      <c r="E46" s="21" t="s">
+      <c r="E46" t="s">
         <v>5</v>
       </c>
       <c r="G46" s="5"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" s="4"/>
-      <c r="E47" s="21" t="s">
+      <c r="E47" t="s">
         <v>49</v>
       </c>
       <c r="G47" s="5"/>
@@ -3277,210 +4570,102 @@
       <c r="B53" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
-      <c r="F53" s="22"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="22"/>
       <c r="I53" s="5"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B54" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="22"/>
       <c r="I54" s="5"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B55" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="22"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
-      <c r="H55" s="22"/>
       <c r="I55" s="5"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C56" s="22"/>
-      <c r="D56" s="22"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="22"/>
-      <c r="G56" s="22"/>
-      <c r="H56" s="22"/>
       <c r="I56" s="5"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C57" s="22"/>
-      <c r="D57" s="22"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
-      <c r="H57" s="22"/>
       <c r="I57" s="5"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="22"/>
-      <c r="G58" s="22"/>
-      <c r="H58" s="22"/>
       <c r="I58" s="5"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C60" s="22"/>
-      <c r="D60" s="22"/>
-      <c r="E60" s="22"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="22"/>
       <c r="I60" s="5"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="22"/>
-      <c r="G61" s="22"/>
-      <c r="H61" s="22"/>
       <c r="I61" s="5"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B62" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="22"/>
-      <c r="D62" s="22"/>
-      <c r="E62" s="22"/>
-      <c r="F62" s="22"/>
-      <c r="G62" s="22"/>
-      <c r="H62" s="22"/>
       <c r="I62" s="5"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B63" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="22"/>
-      <c r="D63" s="22"/>
-      <c r="E63" s="22"/>
-      <c r="F63" s="22"/>
-      <c r="G63" s="22"/>
-      <c r="H63" s="22"/>
       <c r="I63" s="5"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B64" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="22"/>
-      <c r="D64" s="22"/>
-      <c r="E64" s="22"/>
-      <c r="F64" s="22"/>
-      <c r="G64" s="22"/>
-      <c r="H64" s="22"/>
       <c r="I64" s="5"/>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B65" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C65" s="22"/>
-      <c r="D65" s="22"/>
-      <c r="E65" s="22"/>
-      <c r="F65" s="22"/>
-      <c r="G65" s="22"/>
-      <c r="H65" s="22"/>
       <c r="I65" s="5"/>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B66" s="4"/>
-      <c r="C66" s="22"/>
-      <c r="D66" s="22"/>
-      <c r="E66" s="22"/>
-      <c r="F66" s="22"/>
-      <c r="G66" s="22"/>
-      <c r="H66" s="22"/>
       <c r="I66" s="5"/>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B67" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C67" s="22"/>
-      <c r="D67" s="22"/>
-      <c r="E67" s="22"/>
-      <c r="F67" s="22"/>
-      <c r="G67" s="22"/>
-      <c r="H67" s="22"/>
       <c r="I67" s="5"/>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B68" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C68" s="22"/>
-      <c r="D68" s="22"/>
-      <c r="E68" s="22"/>
-      <c r="F68" s="22"/>
-      <c r="G68" s="22"/>
-      <c r="H68" s="22"/>
       <c r="I68" s="5"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C69" s="22"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="22"/>
-      <c r="F69" s="22"/>
-      <c r="G69" s="22"/>
-      <c r="H69" s="22"/>
       <c r="I69" s="5"/>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B70" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C70" s="22"/>
-      <c r="D70" s="22"/>
-      <c r="E70" s="22"/>
-      <c r="F70" s="22"/>
-      <c r="G70" s="22"/>
-      <c r="H70" s="22"/>
       <c r="I70" s="5"/>
       <c r="J70" t="s">
         <v>24</v>
@@ -3493,118 +4678,58 @@
       <c r="B71" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C71" s="22"/>
-      <c r="D71" s="22"/>
-      <c r="E71" s="22"/>
-      <c r="F71" s="22"/>
-      <c r="G71" s="22"/>
-      <c r="H71" s="22"/>
       <c r="I71" s="5"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B72" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="22"/>
-      <c r="G72" s="22"/>
-      <c r="H72" s="22"/>
       <c r="I72" s="5"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C73" s="22"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="22"/>
-      <c r="F73" s="22"/>
-      <c r="G73" s="22"/>
-      <c r="H73" s="22"/>
       <c r="I73" s="5"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B74" s="4"/>
-      <c r="C74" s="22"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="22"/>
-      <c r="F74" s="22"/>
-      <c r="G74" s="22"/>
-      <c r="H74" s="22"/>
       <c r="I74" s="5"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B75" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C75" s="22"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="22"/>
-      <c r="F75" s="22"/>
-      <c r="G75" s="22"/>
-      <c r="H75" s="22"/>
       <c r="I75" s="5"/>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B76" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C76" s="22"/>
-      <c r="D76" s="22"/>
-      <c r="E76" s="22"/>
-      <c r="F76" s="22"/>
-      <c r="G76" s="22"/>
-      <c r="H76" s="22"/>
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B77" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C77" s="22"/>
-      <c r="D77" s="22"/>
-      <c r="E77" s="22"/>
-      <c r="F77" s="22"/>
-      <c r="G77" s="22"/>
-      <c r="H77" s="22"/>
       <c r="I77" s="5"/>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B78" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C78" s="22"/>
-      <c r="D78" s="22"/>
-      <c r="E78" s="22"/>
-      <c r="F78" s="22"/>
-      <c r="G78" s="22"/>
-      <c r="H78" s="22"/>
       <c r="I78" s="5"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B79" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C79" s="22"/>
-      <c r="D79" s="22"/>
-      <c r="E79" s="22"/>
-      <c r="F79" s="22"/>
-      <c r="G79" s="22"/>
-      <c r="H79" s="22"/>
       <c r="I79" s="5"/>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B80" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="22"/>
-      <c r="G80" s="22"/>
-      <c r="H80" s="22"/>
       <c r="I80" s="5"/>
       <c r="J80" t="s">
         <v>24</v>
@@ -3629,4 +4754,1622 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB313400-BA30-8448-9B7E-2E7745B1D5E5}">
+  <dimension ref="A4:T146"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="N97" sqref="N97"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="4"/>
+      <c r="E27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="4"/>
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="4"/>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="4"/>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="4"/>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="4"/>
+      <c r="D34" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="4"/>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="4"/>
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="4"/>
+      <c r="D37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="4"/>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="4"/>
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" s="4"/>
+      <c r="D40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B41" s="4"/>
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B42" s="4"/>
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" s="4"/>
+      <c r="D43" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="9"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="4"/>
+      <c r="E44" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="4"/>
+      <c r="E45" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="4"/>
+      <c r="E46" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="4"/>
+      <c r="E47" t="s">
+        <v>49</v>
+      </c>
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B48" s="4"/>
+      <c r="E48" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G48" s="5"/>
+      <c r="H48" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="8"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B53" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="14"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B54" s="15"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="17"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B55" s="15"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="17"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B56" s="15"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="17"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B57" s="15"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="17"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B58" s="15"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="17"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B59" s="15"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="17"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B60" s="15"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="17"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B61" s="15"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="17"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B62" s="15"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="17"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B63" s="15"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="17"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B64" s="15"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="17"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B65" s="15"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="17"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B66" s="15"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="17"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B67" s="15"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="17"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B68" s="15"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="17"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B69" s="18"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="19"/>
+      <c r="H69" s="20"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B73" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B74" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="22"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="22"/>
+      <c r="I74" s="5"/>
+      <c r="J74" t="s">
+        <v>24</v>
+      </c>
+      <c r="K74" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B75" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C75" s="22"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="22"/>
+      <c r="F75" s="22"/>
+      <c r="G75" s="22"/>
+      <c r="H75" s="22"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B76" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="22"/>
+      <c r="G76" s="22"/>
+      <c r="H76" s="22"/>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B77" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C77" s="22"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="22"/>
+      <c r="F77" s="22"/>
+      <c r="G77" s="22"/>
+      <c r="H77" s="22"/>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B78" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="22"/>
+      <c r="G78" s="22"/>
+      <c r="H78" s="22"/>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B79" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="22"/>
+      <c r="G79" s="22"/>
+      <c r="H79" s="22"/>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B80" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="22"/>
+      <c r="G80" s="22"/>
+      <c r="H80" s="22"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B81" s="4"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="22"/>
+      <c r="G81" s="22"/>
+      <c r="H81" s="22"/>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B82" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="22"/>
+      <c r="H82" s="22"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B83" s="4"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="22"/>
+      <c r="F83" s="22"/>
+      <c r="G83" s="22"/>
+      <c r="H83" s="22"/>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B84" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C84" s="22"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="22"/>
+      <c r="F84" s="22"/>
+      <c r="G84" s="22"/>
+      <c r="H84" s="22"/>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B85" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="22"/>
+      <c r="G85" s="22"/>
+      <c r="H85" s="22"/>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B86" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="22"/>
+      <c r="G86" s="22"/>
+      <c r="H86" s="22"/>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B87" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C87" s="22"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="22"/>
+      <c r="F87" s="22"/>
+      <c r="G87" s="22"/>
+      <c r="H87" s="22"/>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B88" s="4"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="22"/>
+      <c r="F88" s="22"/>
+      <c r="G88" s="22"/>
+      <c r="H88" s="22"/>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B89" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C89" s="22"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="22"/>
+      <c r="F89" s="22"/>
+      <c r="G89" s="22"/>
+      <c r="H89" s="22"/>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B90" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C90" s="22"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="22"/>
+      <c r="F90" s="22"/>
+      <c r="G90" s="22"/>
+      <c r="H90" s="22"/>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B91" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C91" s="22"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="22"/>
+      <c r="F91" s="22"/>
+      <c r="G91" s="22"/>
+      <c r="H91" s="22"/>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B92" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C92" s="22"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="22"/>
+      <c r="F92" s="22"/>
+      <c r="G92" s="22"/>
+      <c r="H92" s="22"/>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B93" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C93" s="22"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="22"/>
+      <c r="F93" s="22"/>
+      <c r="G93" s="22"/>
+      <c r="H93" s="22"/>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B94" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C94" s="22"/>
+      <c r="D94" s="22"/>
+      <c r="E94" s="22"/>
+      <c r="F94" s="22"/>
+      <c r="G94" s="22"/>
+      <c r="H94" s="22"/>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B95" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C95" s="22"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="22"/>
+      <c r="F95" s="22"/>
+      <c r="G95" s="22"/>
+      <c r="H95" s="22"/>
+      <c r="I95" s="5"/>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B96" s="4"/>
+      <c r="C96" s="22"/>
+      <c r="D96" s="22"/>
+      <c r="E96" s="22"/>
+      <c r="F96" s="22"/>
+      <c r="G96" s="22"/>
+      <c r="H96" s="22"/>
+      <c r="I96" s="5"/>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B97" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C97" s="22"/>
+      <c r="D97" s="22"/>
+      <c r="E97" s="22"/>
+      <c r="F97" s="22"/>
+      <c r="G97" s="22"/>
+      <c r="H97" s="22"/>
+      <c r="I97" s="5"/>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B98" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C98" s="22"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="22"/>
+      <c r="F98" s="22"/>
+      <c r="G98" s="22"/>
+      <c r="H98" s="22"/>
+      <c r="I98" s="5"/>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B99" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C99" s="22"/>
+      <c r="D99" s="22"/>
+      <c r="E99" s="22"/>
+      <c r="F99" s="22"/>
+      <c r="G99" s="22"/>
+      <c r="H99" s="22"/>
+      <c r="I99" s="5"/>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B100" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C100" s="22"/>
+      <c r="D100" s="22"/>
+      <c r="E100" s="22"/>
+      <c r="F100" s="22"/>
+      <c r="G100" s="22"/>
+      <c r="H100" s="22"/>
+      <c r="I100" s="5"/>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B101" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C101" s="22"/>
+      <c r="D101" s="22"/>
+      <c r="E101" s="22"/>
+      <c r="F101" s="22"/>
+      <c r="G101" s="22"/>
+      <c r="H101" s="22"/>
+      <c r="I101" s="5"/>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B102" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C102" s="22"/>
+      <c r="D102" s="22"/>
+      <c r="E102" s="22"/>
+      <c r="F102" s="22"/>
+      <c r="G102" s="22"/>
+      <c r="H102" s="22"/>
+      <c r="I102" s="5"/>
+      <c r="J102" t="s">
+        <v>24</v>
+      </c>
+      <c r="K102" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B103" s="4"/>
+      <c r="C103" s="22"/>
+      <c r="D103" s="22"/>
+      <c r="E103" s="22"/>
+      <c r="F103" s="22"/>
+      <c r="G103" s="22"/>
+      <c r="H103" s="22"/>
+      <c r="I103" s="5"/>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B104" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C104" s="22"/>
+      <c r="D104" s="22"/>
+      <c r="E104" s="22"/>
+      <c r="F104" s="22"/>
+      <c r="G104" s="22"/>
+      <c r="H104" s="22"/>
+      <c r="I104" s="5"/>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B105" s="4"/>
+      <c r="C105" s="22"/>
+      <c r="D105" s="22"/>
+      <c r="E105" s="22"/>
+      <c r="F105" s="22"/>
+      <c r="G105" s="22"/>
+      <c r="H105" s="22"/>
+      <c r="I105" s="5"/>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B106" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C106" s="22"/>
+      <c r="D106" s="22"/>
+      <c r="E106" s="22"/>
+      <c r="F106" s="22"/>
+      <c r="G106" s="22"/>
+      <c r="H106" s="22"/>
+      <c r="I106" s="5"/>
+      <c r="J106" t="s">
+        <v>24</v>
+      </c>
+      <c r="K106" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="107" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B107" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C107" s="22"/>
+      <c r="D107" s="22"/>
+      <c r="E107" s="22"/>
+      <c r="F107" s="22"/>
+      <c r="G107" s="22"/>
+      <c r="H107" s="22"/>
+      <c r="I107" s="5"/>
+      <c r="J107" t="s">
+        <v>24</v>
+      </c>
+      <c r="K107" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="108" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B108" s="4"/>
+      <c r="C108" s="22"/>
+      <c r="D108" s="22"/>
+      <c r="E108" s="22"/>
+      <c r="F108" s="22"/>
+      <c r="G108" s="22"/>
+      <c r="H108" s="22"/>
+      <c r="I108" s="5"/>
+    </row>
+    <row r="109" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B109" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C109" s="22"/>
+      <c r="D109" s="22"/>
+      <c r="E109" s="22"/>
+      <c r="F109" s="22"/>
+      <c r="G109" s="22"/>
+      <c r="H109" s="22"/>
+      <c r="I109" s="5"/>
+      <c r="J109" t="s">
+        <v>24</v>
+      </c>
+      <c r="K109" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B110" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C110" s="22"/>
+      <c r="D110" s="22"/>
+      <c r="E110" s="22"/>
+      <c r="F110" s="22"/>
+      <c r="G110" s="22"/>
+      <c r="H110" s="22"/>
+      <c r="I110" s="5"/>
+      <c r="J110" t="s">
+        <v>24</v>
+      </c>
+      <c r="K110" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B111" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C111" s="22"/>
+      <c r="D111" s="22"/>
+      <c r="E111" s="22"/>
+      <c r="F111" s="22"/>
+      <c r="G111" s="22"/>
+      <c r="H111" s="22"/>
+      <c r="I111" s="5"/>
+    </row>
+    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B112" s="4"/>
+      <c r="C112" s="22"/>
+      <c r="D112" s="22"/>
+      <c r="E112" s="22"/>
+      <c r="F112" s="22"/>
+      <c r="G112" s="22"/>
+      <c r="H112" s="22"/>
+      <c r="I112" s="5"/>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B113" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C113" s="22"/>
+      <c r="D113" s="22"/>
+      <c r="E113" s="22"/>
+      <c r="F113" s="22"/>
+      <c r="G113" s="22"/>
+      <c r="H113" s="22"/>
+      <c r="I113" s="5"/>
+      <c r="J113" t="s">
+        <v>24</v>
+      </c>
+      <c r="K113" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B114" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C114" s="22"/>
+      <c r="D114" s="22"/>
+      <c r="E114" s="22"/>
+      <c r="F114" s="22"/>
+      <c r="G114" s="22"/>
+      <c r="H114" s="22"/>
+      <c r="I114" s="5"/>
+      <c r="J114" t="s">
+        <v>24</v>
+      </c>
+      <c r="K114" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B115" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C115" s="22"/>
+      <c r="D115" s="22"/>
+      <c r="E115" s="22"/>
+      <c r="F115" s="22"/>
+      <c r="G115" s="22"/>
+      <c r="H115" s="22"/>
+      <c r="I115" s="5"/>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B116" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C116" s="22"/>
+      <c r="D116" s="22"/>
+      <c r="E116" s="22"/>
+      <c r="F116" s="22"/>
+      <c r="G116" s="22"/>
+      <c r="H116" s="22"/>
+      <c r="I116" s="5"/>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B117" s="4"/>
+      <c r="C117" s="22"/>
+      <c r="D117" s="22"/>
+      <c r="E117" s="22"/>
+      <c r="F117" s="22"/>
+      <c r="G117" s="22"/>
+      <c r="H117" s="22"/>
+      <c r="I117" s="5"/>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B118" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C118" s="22"/>
+      <c r="D118" s="22"/>
+      <c r="E118" s="22"/>
+      <c r="F118" s="22"/>
+      <c r="G118" s="22"/>
+      <c r="H118" s="22"/>
+      <c r="I118" s="5"/>
+      <c r="J118" t="s">
+        <v>24</v>
+      </c>
+      <c r="K118" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B119" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C119" s="22"/>
+      <c r="D119" s="22"/>
+      <c r="E119" s="22"/>
+      <c r="F119" s="22"/>
+      <c r="G119" s="22"/>
+      <c r="H119" s="22"/>
+      <c r="I119" s="5"/>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B120" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C120" s="22"/>
+      <c r="D120" s="22"/>
+      <c r="E120" s="22"/>
+      <c r="F120" s="22"/>
+      <c r="G120" s="22"/>
+      <c r="H120" s="22"/>
+      <c r="I120" s="5"/>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B121" s="4"/>
+      <c r="C121" s="22"/>
+      <c r="D121" s="22"/>
+      <c r="E121" s="22"/>
+      <c r="F121" s="22"/>
+      <c r="G121" s="22"/>
+      <c r="H121" s="22"/>
+      <c r="I121" s="5"/>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B122" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C122" s="22"/>
+      <c r="D122" s="22"/>
+      <c r="E122" s="22"/>
+      <c r="F122" s="22"/>
+      <c r="G122" s="22"/>
+      <c r="H122" s="22"/>
+      <c r="I122" s="5"/>
+      <c r="J122" t="s">
+        <v>24</v>
+      </c>
+      <c r="K122" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B123" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C123" s="22"/>
+      <c r="D123" s="22"/>
+      <c r="E123" s="22"/>
+      <c r="F123" s="22"/>
+      <c r="G123" s="22"/>
+      <c r="H123" s="22"/>
+      <c r="I123" s="5"/>
+      <c r="J123" t="s">
+        <v>24</v>
+      </c>
+      <c r="K123" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B124" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C124" s="22"/>
+      <c r="D124" s="22"/>
+      <c r="E124" s="22"/>
+      <c r="F124" s="22"/>
+      <c r="G124" s="22"/>
+      <c r="H124" s="22"/>
+      <c r="I124" s="5"/>
+      <c r="K124" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B125" s="6"/>
+      <c r="C125" s="7"/>
+      <c r="D125" s="7"/>
+      <c r="E125" s="7"/>
+      <c r="F125" s="7"/>
+      <c r="G125" s="7"/>
+      <c r="H125" s="7"/>
+      <c r="I125" s="8"/>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A128" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B128" s="2"/>
+      <c r="C128" s="2"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+      <c r="H128" s="2"/>
+      <c r="I128" s="2"/>
+      <c r="J128" s="2"/>
+      <c r="K128" s="2"/>
+      <c r="L128" s="2"/>
+      <c r="M128" s="2"/>
+      <c r="N128" s="2"/>
+      <c r="O128" s="2"/>
+      <c r="P128" s="2"/>
+      <c r="Q128" s="2"/>
+      <c r="R128" s="2"/>
+      <c r="S128" s="2"/>
+      <c r="T128" s="3"/>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A129" s="4"/>
+      <c r="B129" s="22"/>
+      <c r="C129" s="22"/>
+      <c r="D129" s="22"/>
+      <c r="E129" s="22"/>
+      <c r="F129" s="22"/>
+      <c r="G129" s="22"/>
+      <c r="H129" s="22"/>
+      <c r="I129" s="22"/>
+      <c r="J129" s="22"/>
+      <c r="K129" s="22"/>
+      <c r="L129" s="22"/>
+      <c r="M129" s="22"/>
+      <c r="N129" s="22"/>
+      <c r="O129" s="22"/>
+      <c r="P129" s="22"/>
+      <c r="Q129" s="22"/>
+      <c r="R129" s="22"/>
+      <c r="S129" s="22"/>
+      <c r="T129" s="5"/>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A130" s="4"/>
+      <c r="B130" s="22"/>
+      <c r="C130" s="22"/>
+      <c r="D130" s="22"/>
+      <c r="E130" s="22"/>
+      <c r="F130" s="22"/>
+      <c r="G130" s="22"/>
+      <c r="H130" s="22"/>
+      <c r="I130" s="22"/>
+      <c r="J130" s="22"/>
+      <c r="K130" s="22"/>
+      <c r="L130" s="22"/>
+      <c r="M130" s="22"/>
+      <c r="N130" s="22"/>
+      <c r="O130" s="22"/>
+      <c r="P130" s="22"/>
+      <c r="Q130" s="22"/>
+      <c r="R130" s="22"/>
+      <c r="S130" s="22"/>
+      <c r="T130" s="5"/>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A131" s="4"/>
+      <c r="B131" s="22"/>
+      <c r="C131" s="22"/>
+      <c r="D131" s="22"/>
+      <c r="E131" s="22"/>
+      <c r="F131" s="22"/>
+      <c r="G131" s="22"/>
+      <c r="H131" s="22"/>
+      <c r="I131" s="22"/>
+      <c r="J131" s="22"/>
+      <c r="K131" s="22"/>
+      <c r="L131" s="22"/>
+      <c r="M131" s="22"/>
+      <c r="N131" s="22"/>
+      <c r="O131" s="22"/>
+      <c r="P131" s="22"/>
+      <c r="Q131" s="22"/>
+      <c r="R131" s="22"/>
+      <c r="S131" s="22"/>
+      <c r="T131" s="5"/>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A132" s="4"/>
+      <c r="B132" s="22"/>
+      <c r="C132" s="22"/>
+      <c r="D132" s="22"/>
+      <c r="E132" s="22"/>
+      <c r="F132" s="22"/>
+      <c r="G132" s="22"/>
+      <c r="H132" s="22"/>
+      <c r="I132" s="22"/>
+      <c r="J132" s="22"/>
+      <c r="K132" s="22"/>
+      <c r="L132" s="22"/>
+      <c r="M132" s="22"/>
+      <c r="N132" s="22"/>
+      <c r="O132" s="22"/>
+      <c r="P132" s="22"/>
+      <c r="Q132" s="22"/>
+      <c r="R132" s="22"/>
+      <c r="S132" s="22"/>
+      <c r="T132" s="5"/>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A133" s="4"/>
+      <c r="B133" s="22"/>
+      <c r="C133" s="22"/>
+      <c r="D133" s="22"/>
+      <c r="E133" s="22"/>
+      <c r="F133" s="22"/>
+      <c r="G133" s="22"/>
+      <c r="H133" s="22"/>
+      <c r="I133" s="22"/>
+      <c r="J133" s="22"/>
+      <c r="K133" s="22"/>
+      <c r="L133" s="22"/>
+      <c r="M133" s="22"/>
+      <c r="N133" s="22"/>
+      <c r="O133" s="22"/>
+      <c r="P133" s="22"/>
+      <c r="Q133" s="22"/>
+      <c r="R133" s="22"/>
+      <c r="S133" s="22"/>
+      <c r="T133" s="5"/>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A134" s="4"/>
+      <c r="B134" s="22"/>
+      <c r="C134" s="22"/>
+      <c r="D134" s="22"/>
+      <c r="E134" s="22"/>
+      <c r="F134" s="22"/>
+      <c r="G134" s="22"/>
+      <c r="H134" s="22"/>
+      <c r="I134" s="22"/>
+      <c r="J134" s="22"/>
+      <c r="K134" s="22"/>
+      <c r="L134" s="22"/>
+      <c r="M134" s="22"/>
+      <c r="N134" s="22"/>
+      <c r="O134" s="22"/>
+      <c r="P134" s="22"/>
+      <c r="Q134" s="22"/>
+      <c r="R134" s="22"/>
+      <c r="S134" s="22"/>
+      <c r="T134" s="5"/>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A135" s="4"/>
+      <c r="B135" s="22"/>
+      <c r="C135" s="22"/>
+      <c r="D135" s="22"/>
+      <c r="E135" s="22"/>
+      <c r="F135" s="22"/>
+      <c r="G135" s="22"/>
+      <c r="H135" s="22"/>
+      <c r="I135" s="22"/>
+      <c r="J135" s="22"/>
+      <c r="K135" s="22"/>
+      <c r="L135" s="22"/>
+      <c r="M135" s="22"/>
+      <c r="N135" s="22"/>
+      <c r="O135" s="22"/>
+      <c r="P135" s="22"/>
+      <c r="Q135" s="22"/>
+      <c r="R135" s="22"/>
+      <c r="S135" s="22"/>
+      <c r="T135" s="5"/>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A136" s="4"/>
+      <c r="B136" s="22"/>
+      <c r="C136" s="22"/>
+      <c r="D136" s="22"/>
+      <c r="E136" s="22"/>
+      <c r="F136" s="22"/>
+      <c r="G136" s="22"/>
+      <c r="H136" s="22"/>
+      <c r="I136" s="22"/>
+      <c r="J136" s="22"/>
+      <c r="K136" s="22"/>
+      <c r="L136" s="22"/>
+      <c r="M136" s="22"/>
+      <c r="N136" s="22"/>
+      <c r="O136" s="22"/>
+      <c r="P136" s="22"/>
+      <c r="Q136" s="22"/>
+      <c r="R136" s="22"/>
+      <c r="S136" s="22"/>
+      <c r="T136" s="5"/>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A137" s="4"/>
+      <c r="B137" s="22"/>
+      <c r="C137" s="22"/>
+      <c r="D137" s="22"/>
+      <c r="E137" s="22"/>
+      <c r="F137" s="22"/>
+      <c r="G137" s="22"/>
+      <c r="H137" s="22"/>
+      <c r="I137" s="22"/>
+      <c r="J137" s="22"/>
+      <c r="K137" s="22"/>
+      <c r="L137" s="22"/>
+      <c r="M137" s="22"/>
+      <c r="N137" s="22"/>
+      <c r="O137" s="22"/>
+      <c r="P137" s="22"/>
+      <c r="Q137" s="22"/>
+      <c r="R137" s="22"/>
+      <c r="S137" s="22"/>
+      <c r="T137" s="5"/>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A138" s="4"/>
+      <c r="B138" s="22"/>
+      <c r="C138" s="22"/>
+      <c r="D138" s="22"/>
+      <c r="E138" s="22"/>
+      <c r="F138" s="22"/>
+      <c r="G138" s="22"/>
+      <c r="H138" s="22"/>
+      <c r="I138" s="22"/>
+      <c r="J138" s="22"/>
+      <c r="K138" s="22"/>
+      <c r="L138" s="22"/>
+      <c r="M138" s="22"/>
+      <c r="N138" s="22"/>
+      <c r="O138" s="22"/>
+      <c r="P138" s="22"/>
+      <c r="Q138" s="22"/>
+      <c r="R138" s="22"/>
+      <c r="S138" s="22"/>
+      <c r="T138" s="5"/>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A139" s="4"/>
+      <c r="B139" s="22"/>
+      <c r="C139" s="22"/>
+      <c r="D139" s="22"/>
+      <c r="E139" s="22"/>
+      <c r="F139" s="22"/>
+      <c r="G139" s="22"/>
+      <c r="H139" s="22"/>
+      <c r="I139" s="22"/>
+      <c r="J139" s="22"/>
+      <c r="K139" s="22"/>
+      <c r="L139" s="22"/>
+      <c r="M139" s="22"/>
+      <c r="N139" s="22"/>
+      <c r="O139" s="22"/>
+      <c r="P139" s="22"/>
+      <c r="Q139" s="22"/>
+      <c r="R139" s="22"/>
+      <c r="S139" s="22"/>
+      <c r="T139" s="5"/>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A140" s="4"/>
+      <c r="B140" s="22"/>
+      <c r="C140" s="22"/>
+      <c r="D140" s="22"/>
+      <c r="E140" s="22"/>
+      <c r="F140" s="22"/>
+      <c r="G140" s="22"/>
+      <c r="H140" s="22"/>
+      <c r="I140" s="22"/>
+      <c r="J140" s="22"/>
+      <c r="K140" s="22"/>
+      <c r="L140" s="22"/>
+      <c r="M140" s="22"/>
+      <c r="N140" s="22"/>
+      <c r="O140" s="22"/>
+      <c r="P140" s="22"/>
+      <c r="Q140" s="22"/>
+      <c r="R140" s="22"/>
+      <c r="S140" s="22"/>
+      <c r="T140" s="5"/>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A141" s="4"/>
+      <c r="B141" s="22"/>
+      <c r="C141" s="22"/>
+      <c r="D141" s="22"/>
+      <c r="E141" s="22"/>
+      <c r="F141" s="22"/>
+      <c r="G141" s="22"/>
+      <c r="H141" s="22"/>
+      <c r="I141" s="22"/>
+      <c r="J141" s="22"/>
+      <c r="K141" s="22"/>
+      <c r="L141" s="22"/>
+      <c r="M141" s="22"/>
+      <c r="N141" s="22"/>
+      <c r="O141" s="22"/>
+      <c r="P141" s="22"/>
+      <c r="Q141" s="22"/>
+      <c r="R141" s="22"/>
+      <c r="S141" s="22"/>
+      <c r="T141" s="5"/>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A142" s="4"/>
+      <c r="B142" s="22"/>
+      <c r="C142" s="22"/>
+      <c r="D142" s="22"/>
+      <c r="E142" s="22"/>
+      <c r="F142" s="22"/>
+      <c r="G142" s="22"/>
+      <c r="H142" s="22"/>
+      <c r="I142" s="22"/>
+      <c r="J142" s="22"/>
+      <c r="K142" s="22"/>
+      <c r="L142" s="22"/>
+      <c r="M142" s="22"/>
+      <c r="N142" s="22"/>
+      <c r="O142" s="22"/>
+      <c r="P142" s="22"/>
+      <c r="Q142" s="22"/>
+      <c r="R142" s="22"/>
+      <c r="S142" s="22"/>
+      <c r="T142" s="5"/>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A143" s="4"/>
+      <c r="B143" s="22"/>
+      <c r="C143" s="22"/>
+      <c r="D143" s="22"/>
+      <c r="E143" s="22"/>
+      <c r="F143" s="22"/>
+      <c r="G143" s="22"/>
+      <c r="H143" s="22"/>
+      <c r="I143" s="22"/>
+      <c r="J143" s="22"/>
+      <c r="K143" s="22"/>
+      <c r="L143" s="22"/>
+      <c r="M143" s="22"/>
+      <c r="N143" s="22"/>
+      <c r="O143" s="22"/>
+      <c r="P143" s="22"/>
+      <c r="Q143" s="22"/>
+      <c r="R143" s="22"/>
+      <c r="S143" s="22"/>
+      <c r="T143" s="5"/>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A144" s="4"/>
+      <c r="B144" s="22"/>
+      <c r="C144" s="22"/>
+      <c r="D144" s="22"/>
+      <c r="E144" s="22"/>
+      <c r="F144" s="22"/>
+      <c r="G144" s="22"/>
+      <c r="H144" s="22"/>
+      <c r="I144" s="22"/>
+      <c r="J144" s="22"/>
+      <c r="K144" s="22"/>
+      <c r="L144" s="22"/>
+      <c r="M144" s="22"/>
+      <c r="N144" s="22"/>
+      <c r="O144" s="22"/>
+      <c r="P144" s="22"/>
+      <c r="Q144" s="22"/>
+      <c r="R144" s="22"/>
+      <c r="S144" s="22"/>
+      <c r="T144" s="5"/>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A145" s="4"/>
+      <c r="B145" s="22"/>
+      <c r="C145" s="22"/>
+      <c r="D145" s="22"/>
+      <c r="E145" s="22"/>
+      <c r="F145" s="22"/>
+      <c r="G145" s="22"/>
+      <c r="H145" s="22"/>
+      <c r="I145" s="22"/>
+      <c r="J145" s="22"/>
+      <c r="K145" s="22"/>
+      <c r="L145" s="22"/>
+      <c r="M145" s="22"/>
+      <c r="N145" s="22"/>
+      <c r="O145" s="22"/>
+      <c r="P145" s="22"/>
+      <c r="Q145" s="22"/>
+      <c r="R145" s="22"/>
+      <c r="S145" s="22"/>
+      <c r="T145" s="5"/>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A146" s="6"/>
+      <c r="B146" s="7"/>
+      <c r="C146" s="7"/>
+      <c r="D146" s="7"/>
+      <c r="E146" s="7"/>
+      <c r="F146" s="7"/>
+      <c r="G146" s="7"/>
+      <c r="H146" s="7"/>
+      <c r="I146" s="7"/>
+      <c r="J146" s="7"/>
+      <c r="K146" s="7"/>
+      <c r="L146" s="7"/>
+      <c r="M146" s="7"/>
+      <c r="N146" s="7"/>
+      <c r="O146" s="7"/>
+      <c r="P146" s="7"/>
+      <c r="Q146" s="7"/>
+      <c r="R146" s="7"/>
+      <c r="S146" s="7"/>
+      <c r="T146" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B53:H69"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Practice 02 - Solution 02
</commit_message>
<xml_diff>
--- a/me/2.Asynchronous-ProgrammingChương-Asynchronous-Programming/6.Bai-tap-thuc-hanh-so-01-02.xlsx
+++ b/me/2.Asynchronous-ProgrammingChương-Asynchronous-Programming/6.Bai-tap-thuc-hanh-so-01-02.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/javascript_advance/me/2.Asynchronous-ProgrammingChương-Asynchronous-Programming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242E6D0D-8397-6E4C-A512-8022BEA70271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE01FFF6-645D-0B4A-B727-A1410DA152E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="1740" windowWidth="31740" windowHeight="18760" activeTab="3" xr2:uid="{7676CE1B-4587-7A49-84A8-63238B5A3602}"/>
+    <workbookView xWindow="2240" yWindow="1740" windowWidth="31740" windowHeight="18760" activeTab="4" xr2:uid="{7676CE1B-4587-7A49-84A8-63238B5A3602}"/>
   </bookViews>
   <sheets>
     <sheet name="Practice 01" sheetId="1" r:id="rId1"/>
     <sheet name="Practice 01 - Solution" sheetId="2" r:id="rId2"/>
     <sheet name="Practice 02" sheetId="3" r:id="rId3"/>
     <sheet name="Practice 02 - Solution 01" sheetId="4" r:id="rId4"/>
+    <sheet name="Practice 02 - Solution 02" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="152">
   <si>
     <t>構成</t>
   </si>
@@ -958,6 +959,333 @@
   </si>
   <si>
     <t>Check browser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  let callback = null;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if (callback !== null) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      callback(data); // cbFn(res)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    } else {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if (res !== null) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      callback = cbFn;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  fnGetData2(function(res2){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    console.log(res2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    fnGetData3(function(res3){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      console.log(res3)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mình có 2 function được gọi tại 2 thời điểm khác nhau đó là function </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>getData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> và function </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>call back</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ở trong hàm </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>fakeGetData</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">res khác null có nghĩa là hàm fakeGetData đã chạy xong, chỉ khi nào fakeGetData chạy xong thì </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">data </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>mới có giá trị</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> và data được gán cho </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>res</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">hàm fakeGetData chưa được chạy tức là data chưa có giá trị thì mình sẽ chờ mà chưa gọi hàm cbFn ngay mà mình sẽ lưu tạm thời hàm này vào biến </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>callback</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Bản thân 1 hàm trong JS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">nó là dạng First Class Object(First Class Function) nên mình có thể truyền vào hàm khác như 1 tham số, có thể return từ 1 hàm khác hoặc cũng có thể </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>lưu lại như 1 biến</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kiểm tra nếu như </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>callback</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> khác null nghĩa là callback là 1 function. Nếu callback là 1 function thì có nghĩa là hàm </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>getData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> đã được chạy vì getData đã được chạy rồi thì callback mới được gán </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>callback = cbFn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>. Trường</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trường hợp này </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>callback</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> là </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> đồng nghĩa với việc function </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>getData</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> chưa được chạy, trường hợp này mình tiến hành </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>lưu lại data vào res</t>
+    </r>
+  </si>
+  <si>
+    <t>hợp này mình sẽ gửi data ra bên ngoài luôn từ bước này bằng cách gọi hàm callback hay cũng chính là hàm cbFn</t>
+  </si>
+  <si>
+    <t>res khác null nên mình tiến hành gọi hàm call back cbFn() ở đây</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Gọi hàm nhưng sau khi </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>setTimeout()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> chạy xong thì mới có mới có dữ liệu </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>res1</t>
+    </r>
+  </si>
+  <si>
+    <t>API 1 chạy lâu nhất nên sau khi res1 được in ra thì res2 và res3 cũng được in ra luôn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 API được gọi đồng thời cùng 1 lúc do đó toàn bộ chương trình chỉ mất tối đa là hơn 4s thôi bởi vì nó lợi dụng cơ chế của Web APIs để xử dụng tính năng Timer và chạy đồng thời cùng 1 lúc mà không cần phải chờ gì cả mà nó chỉ phụ thuộc </t>
+  </si>
+  <si>
+    <t>vào cái lâu nhất thôi</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1111,6 +1439,8 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1138,9 +1468,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2510,6 +2837,897 @@
         <a:xfrm flipH="1">
           <a:off x="1257300" y="24968200"/>
           <a:ext cx="495300" cy="4216400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4857BC4-6DA1-F007-87EE-6989FA7203FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="977900" y="24765000"/>
+          <a:ext cx="15189200" cy="7594600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDC3F628-534F-80A3-1731-91C00EB64934}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1041400" y="19723100"/>
+          <a:ext cx="11582400" cy="2501900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AEBD66F-2383-B157-43B9-AECBC2D27169}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2247900" y="18072100"/>
+          <a:ext cx="11747500" cy="1498600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFEEAA31-010E-41D3-910E-2C03D6A78266}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1587500" y="18884900"/>
+          <a:ext cx="12827000" cy="901700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A2C9EEA-AD72-597C-F753-82610401FCEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1701800" y="19685000"/>
+          <a:ext cx="850900" cy="2565400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1FF69FE-AE9F-2C27-9DA8-C2F20650708E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2095500" y="18262600"/>
+          <a:ext cx="18135600" cy="2197100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3888826-B920-9099-8EEF-DDE1FFDC93E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2146300" y="18262600"/>
+          <a:ext cx="13246100" cy="1308100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2037D1FA-79C5-3612-6707-7E3433933399}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2209800" y="18681700"/>
+          <a:ext cx="10109200" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BD289AD-AE20-9015-BF00-1C240D912041}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1041400" y="10744200"/>
+          <a:ext cx="406400" cy="7213600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23DFAF33-B596-8D77-463B-24967E038553}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1828800" y="12763500"/>
+          <a:ext cx="7975600" cy="9486900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4EECCEE-8A41-D274-B5C8-0A0C1D20FB0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1968500" y="22326600"/>
+          <a:ext cx="10985500" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>113740</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB059FE9-6E97-D8C0-1595-5FC1C1F41C0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="977900" y="33261300"/>
+          <a:ext cx="15049500" cy="4647640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>213</xdr:row>
+      <xdr:rowOff>50240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{960CCD7A-E662-56D8-7ABE-AADEFBB87239}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="952500" y="38481000"/>
+          <a:ext cx="15049500" cy="4647640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B1EB603-510D-F973-34B2-D25DFA2DA428}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="965200" y="33070800"/>
+          <a:ext cx="368300" cy="3606800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>189</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>209</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Arrow Connector 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDA336C2-EBE5-A51F-AEFB-4FB55DCB73A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1181100" y="38366700"/>
+          <a:ext cx="1701800" cy="4025900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Arrow Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D97E89A-524E-39AC-EFA4-50AF8A78DDAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1460500" y="33274000"/>
+          <a:ext cx="3213100" cy="3657600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Straight Arrow Connector 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D7BEBE8-D325-C24B-AD90-2628174D9D60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4711700" y="33096200"/>
+          <a:ext cx="1587500" cy="3822700"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3165,159 +4383,159 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="14"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="16"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="15"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="17"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="19"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="15"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="17"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="19"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B53" s="15"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="17"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="19"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B54" s="15"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="17"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="19"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="15"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="17"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="19"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="15"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="19"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="15"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="17"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="19"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B58" s="15"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="17"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="19"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B59" s="15"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="17"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="19"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B60" s="15"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="17"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="19"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B61" s="15"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="17"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="19"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="15"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="17"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="19"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="15"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="17"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="19"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="15"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="17"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="19"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B65" s="15"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="17"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="19"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B66" s="18"/>
-      <c r="C66" s="19"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="19"/>
-      <c r="H66" s="20"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="22"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B67" s="10"/>
@@ -3826,159 +5044,159 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="14"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="16"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B54" s="15"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="17"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="19"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="15"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="17"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="19"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="15"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="19"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="15"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="17"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="19"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B58" s="15"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="17"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="19"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B59" s="15"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="17"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="19"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B60" s="15"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="17"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="19"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B61" s="15"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="17"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="19"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="15"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="17"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="19"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="15"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="17"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="19"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="15"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="17"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="19"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B65" s="15"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="17"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="19"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B66" s="15"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="17"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="19"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B67" s="15"/>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="17"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="19"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B68" s="15"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
-      <c r="H68" s="17"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="19"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B69" s="18"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="19"/>
-      <c r="H69" s="20"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="22"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -4760,8 +5978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB313400-BA30-8448-9B7E-2E7745B1D5E5}">
   <dimension ref="A4:T146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="N97" sqref="N97"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5057,7 +6275,7 @@
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="4"/>
-      <c r="E45" s="21" t="s">
+      <c r="E45" t="s">
         <v>10</v>
       </c>
       <c r="G45" s="5"/>
@@ -5103,159 +6321,159 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="14"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="16"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B54" s="15"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="17"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="19"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="15"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="17"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="19"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="15"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="19"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="15"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="17"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="19"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B58" s="15"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="17"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="19"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B59" s="15"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="17"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="19"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B60" s="15"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="17"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="19"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B61" s="15"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="17"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="19"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="15"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="17"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="19"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="15"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="17"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="19"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="15"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="17"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="19"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B65" s="15"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="17"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="19"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B66" s="15"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="16"/>
-      <c r="H66" s="17"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
+      <c r="H66" s="19"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B67" s="15"/>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="16"/>
-      <c r="H67" s="17"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="19"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B68" s="15"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
-      <c r="H68" s="17"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="19"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B69" s="18"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="19"/>
-      <c r="H69" s="20"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="22"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -5278,12 +6496,6 @@
       <c r="B74" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C74" s="22"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="22"/>
-      <c r="F74" s="22"/>
-      <c r="G74" s="22"/>
-      <c r="H74" s="22"/>
       <c r="I74" s="5"/>
       <c r="J74" t="s">
         <v>24</v>
@@ -5296,328 +6508,160 @@
       <c r="B75" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C75" s="22"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="22"/>
-      <c r="F75" s="22"/>
-      <c r="G75" s="22"/>
-      <c r="H75" s="22"/>
       <c r="I75" s="5"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B76" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C76" s="22"/>
-      <c r="D76" s="22"/>
-      <c r="E76" s="22"/>
-      <c r="F76" s="22"/>
-      <c r="G76" s="22"/>
-      <c r="H76" s="22"/>
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B77" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C77" s="22"/>
-      <c r="D77" s="22"/>
-      <c r="E77" s="22"/>
-      <c r="F77" s="22"/>
-      <c r="G77" s="22"/>
-      <c r="H77" s="22"/>
       <c r="I77" s="5"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B78" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C78" s="22"/>
-      <c r="D78" s="22"/>
-      <c r="E78" s="22"/>
-      <c r="F78" s="22"/>
-      <c r="G78" s="22"/>
-      <c r="H78" s="22"/>
       <c r="I78" s="5"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B79" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C79" s="22"/>
-      <c r="D79" s="22"/>
-      <c r="E79" s="22"/>
-      <c r="F79" s="22"/>
-      <c r="G79" s="22"/>
-      <c r="H79" s="22"/>
       <c r="I79" s="5"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B80" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="22"/>
-      <c r="F80" s="22"/>
-      <c r="G80" s="22"/>
-      <c r="H80" s="22"/>
       <c r="I80" s="5"/>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B81" s="4"/>
-      <c r="C81" s="22"/>
-      <c r="D81" s="22"/>
-      <c r="E81" s="22"/>
-      <c r="F81" s="22"/>
-      <c r="G81" s="22"/>
-      <c r="H81" s="22"/>
       <c r="I81" s="5"/>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B82" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C82" s="22"/>
-      <c r="D82" s="22"/>
-      <c r="E82" s="22"/>
-      <c r="F82" s="22"/>
-      <c r="G82" s="22"/>
-      <c r="H82" s="22"/>
       <c r="I82" s="5"/>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B83" s="4"/>
-      <c r="C83" s="22"/>
-      <c r="D83" s="22"/>
-      <c r="E83" s="22"/>
-      <c r="F83" s="22"/>
-      <c r="G83" s="22"/>
-      <c r="H83" s="22"/>
       <c r="I83" s="5"/>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C84" s="22"/>
-      <c r="D84" s="22"/>
-      <c r="E84" s="22"/>
-      <c r="F84" s="22"/>
-      <c r="G84" s="22"/>
-      <c r="H84" s="22"/>
       <c r="I84" s="5"/>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B85" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C85" s="22"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="22"/>
-      <c r="G85" s="22"/>
-      <c r="H85" s="22"/>
       <c r="I85" s="5"/>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B86" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C86" s="22"/>
-      <c r="D86" s="22"/>
-      <c r="E86" s="22"/>
-      <c r="F86" s="22"/>
-      <c r="G86" s="22"/>
-      <c r="H86" s="22"/>
       <c r="I86" s="5"/>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B87" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C87" s="22"/>
-      <c r="D87" s="22"/>
-      <c r="E87" s="22"/>
-      <c r="F87" s="22"/>
-      <c r="G87" s="22"/>
-      <c r="H87" s="22"/>
       <c r="I87" s="5"/>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B88" s="4"/>
-      <c r="C88" s="22"/>
-      <c r="D88" s="22"/>
-      <c r="E88" s="22"/>
-      <c r="F88" s="22"/>
-      <c r="G88" s="22"/>
-      <c r="H88" s="22"/>
       <c r="I88" s="5"/>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B89" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C89" s="22"/>
-      <c r="D89" s="22"/>
-      <c r="E89" s="22"/>
-      <c r="F89" s="22"/>
-      <c r="G89" s="22"/>
-      <c r="H89" s="22"/>
       <c r="I89" s="5"/>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B90" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C90" s="22"/>
-      <c r="D90" s="22"/>
-      <c r="E90" s="22"/>
-      <c r="F90" s="22"/>
-      <c r="G90" s="22"/>
-      <c r="H90" s="22"/>
       <c r="I90" s="5"/>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B91" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C91" s="22"/>
-      <c r="D91" s="22"/>
-      <c r="E91" s="22"/>
-      <c r="F91" s="22"/>
-      <c r="G91" s="22"/>
-      <c r="H91" s="22"/>
       <c r="I91" s="5"/>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B92" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C92" s="22"/>
-      <c r="D92" s="22"/>
-      <c r="E92" s="22"/>
-      <c r="F92" s="22"/>
-      <c r="G92" s="22"/>
-      <c r="H92" s="22"/>
       <c r="I92" s="5"/>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B93" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C93" s="22"/>
-      <c r="D93" s="22"/>
-      <c r="E93" s="22"/>
-      <c r="F93" s="22"/>
-      <c r="G93" s="22"/>
-      <c r="H93" s="22"/>
       <c r="I93" s="5"/>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B94" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C94" s="22"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="22"/>
-      <c r="F94" s="22"/>
-      <c r="G94" s="22"/>
-      <c r="H94" s="22"/>
       <c r="I94" s="5"/>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B95" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C95" s="22"/>
-      <c r="D95" s="22"/>
-      <c r="E95" s="22"/>
-      <c r="F95" s="22"/>
-      <c r="G95" s="22"/>
-      <c r="H95" s="22"/>
       <c r="I95" s="5"/>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B96" s="4"/>
-      <c r="C96" s="22"/>
-      <c r="D96" s="22"/>
-      <c r="E96" s="22"/>
-      <c r="F96" s="22"/>
-      <c r="G96" s="22"/>
-      <c r="H96" s="22"/>
       <c r="I96" s="5"/>
     </row>
     <row r="97" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B97" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C97" s="22"/>
-      <c r="D97" s="22"/>
-      <c r="E97" s="22"/>
-      <c r="F97" s="22"/>
-      <c r="G97" s="22"/>
-      <c r="H97" s="22"/>
       <c r="I97" s="5"/>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B98" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C98" s="22"/>
-      <c r="D98" s="22"/>
-      <c r="E98" s="22"/>
-      <c r="F98" s="22"/>
-      <c r="G98" s="22"/>
-      <c r="H98" s="22"/>
       <c r="I98" s="5"/>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B99" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C99" s="22"/>
-      <c r="D99" s="22"/>
-      <c r="E99" s="22"/>
-      <c r="F99" s="22"/>
-      <c r="G99" s="22"/>
-      <c r="H99" s="22"/>
       <c r="I99" s="5"/>
     </row>
     <row r="100" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B100" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C100" s="22"/>
-      <c r="D100" s="22"/>
-      <c r="E100" s="22"/>
-      <c r="F100" s="22"/>
-      <c r="G100" s="22"/>
-      <c r="H100" s="22"/>
       <c r="I100" s="5"/>
     </row>
     <row r="101" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B101" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C101" s="22"/>
-      <c r="D101" s="22"/>
-      <c r="E101" s="22"/>
-      <c r="F101" s="22"/>
-      <c r="G101" s="22"/>
-      <c r="H101" s="22"/>
       <c r="I101" s="5"/>
     </row>
     <row r="102" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B102" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C102" s="22"/>
-      <c r="D102" s="22"/>
-      <c r="E102" s="22"/>
-      <c r="F102" s="22"/>
-      <c r="G102" s="22"/>
-      <c r="H102" s="22"/>
       <c r="I102" s="5"/>
       <c r="J102" t="s">
         <v>24</v>
@@ -5628,46 +6672,22 @@
     </row>
     <row r="103" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B103" s="4"/>
-      <c r="C103" s="22"/>
-      <c r="D103" s="22"/>
-      <c r="E103" s="22"/>
-      <c r="F103" s="22"/>
-      <c r="G103" s="22"/>
-      <c r="H103" s="22"/>
       <c r="I103" s="5"/>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B104" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C104" s="22"/>
-      <c r="D104" s="22"/>
-      <c r="E104" s="22"/>
-      <c r="F104" s="22"/>
-      <c r="G104" s="22"/>
-      <c r="H104" s="22"/>
       <c r="I104" s="5"/>
     </row>
     <row r="105" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B105" s="4"/>
-      <c r="C105" s="22"/>
-      <c r="D105" s="22"/>
-      <c r="E105" s="22"/>
-      <c r="F105" s="22"/>
-      <c r="G105" s="22"/>
-      <c r="H105" s="22"/>
       <c r="I105" s="5"/>
     </row>
     <row r="106" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B106" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C106" s="22"/>
-      <c r="D106" s="22"/>
-      <c r="E106" s="22"/>
-      <c r="F106" s="22"/>
-      <c r="G106" s="22"/>
-      <c r="H106" s="22"/>
       <c r="I106" s="5"/>
       <c r="J106" t="s">
         <v>24</v>
@@ -5680,12 +6700,6 @@
       <c r="B107" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C107" s="22"/>
-      <c r="D107" s="22"/>
-      <c r="E107" s="22"/>
-      <c r="F107" s="22"/>
-      <c r="G107" s="22"/>
-      <c r="H107" s="22"/>
       <c r="I107" s="5"/>
       <c r="J107" t="s">
         <v>24</v>
@@ -5696,24 +6710,12 @@
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B108" s="4"/>
-      <c r="C108" s="22"/>
-      <c r="D108" s="22"/>
-      <c r="E108" s="22"/>
-      <c r="F108" s="22"/>
-      <c r="G108" s="22"/>
-      <c r="H108" s="22"/>
       <c r="I108" s="5"/>
     </row>
     <row r="109" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B109" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C109" s="22"/>
-      <c r="D109" s="22"/>
-      <c r="E109" s="22"/>
-      <c r="F109" s="22"/>
-      <c r="G109" s="22"/>
-      <c r="H109" s="22"/>
       <c r="I109" s="5"/>
       <c r="J109" t="s">
         <v>24</v>
@@ -5726,12 +6728,6 @@
       <c r="B110" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C110" s="22"/>
-      <c r="D110" s="22"/>
-      <c r="E110" s="22"/>
-      <c r="F110" s="22"/>
-      <c r="G110" s="22"/>
-      <c r="H110" s="22"/>
       <c r="I110" s="5"/>
       <c r="J110" t="s">
         <v>24</v>
@@ -5744,34 +6740,16 @@
       <c r="B111" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C111" s="22"/>
-      <c r="D111" s="22"/>
-      <c r="E111" s="22"/>
-      <c r="F111" s="22"/>
-      <c r="G111" s="22"/>
-      <c r="H111" s="22"/>
       <c r="I111" s="5"/>
     </row>
     <row r="112" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B112" s="4"/>
-      <c r="C112" s="22"/>
-      <c r="D112" s="22"/>
-      <c r="E112" s="22"/>
-      <c r="F112" s="22"/>
-      <c r="G112" s="22"/>
-      <c r="H112" s="22"/>
       <c r="I112" s="5"/>
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B113" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C113" s="22"/>
-      <c r="D113" s="22"/>
-      <c r="E113" s="22"/>
-      <c r="F113" s="22"/>
-      <c r="G113" s="22"/>
-      <c r="H113" s="22"/>
       <c r="I113" s="5"/>
       <c r="J113" t="s">
         <v>24</v>
@@ -5784,12 +6762,6 @@
       <c r="B114" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C114" s="22"/>
-      <c r="D114" s="22"/>
-      <c r="E114" s="22"/>
-      <c r="F114" s="22"/>
-      <c r="G114" s="22"/>
-      <c r="H114" s="22"/>
       <c r="I114" s="5"/>
       <c r="J114" t="s">
         <v>24</v>
@@ -5802,46 +6774,22 @@
       <c r="B115" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C115" s="22"/>
-      <c r="D115" s="22"/>
-      <c r="E115" s="22"/>
-      <c r="F115" s="22"/>
-      <c r="G115" s="22"/>
-      <c r="H115" s="22"/>
       <c r="I115" s="5"/>
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B116" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C116" s="22"/>
-      <c r="D116" s="22"/>
-      <c r="E116" s="22"/>
-      <c r="F116" s="22"/>
-      <c r="G116" s="22"/>
-      <c r="H116" s="22"/>
       <c r="I116" s="5"/>
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B117" s="4"/>
-      <c r="C117" s="22"/>
-      <c r="D117" s="22"/>
-      <c r="E117" s="22"/>
-      <c r="F117" s="22"/>
-      <c r="G117" s="22"/>
-      <c r="H117" s="22"/>
       <c r="I117" s="5"/>
     </row>
     <row r="118" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B118" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C118" s="22"/>
-      <c r="D118" s="22"/>
-      <c r="E118" s="22"/>
-      <c r="F118" s="22"/>
-      <c r="G118" s="22"/>
-      <c r="H118" s="22"/>
       <c r="I118" s="5"/>
       <c r="J118" t="s">
         <v>24</v>
@@ -5854,46 +6802,22 @@
       <c r="B119" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C119" s="22"/>
-      <c r="D119" s="22"/>
-      <c r="E119" s="22"/>
-      <c r="F119" s="22"/>
-      <c r="G119" s="22"/>
-      <c r="H119" s="22"/>
       <c r="I119" s="5"/>
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B120" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C120" s="22"/>
-      <c r="D120" s="22"/>
-      <c r="E120" s="22"/>
-      <c r="F120" s="22"/>
-      <c r="G120" s="22"/>
-      <c r="H120" s="22"/>
       <c r="I120" s="5"/>
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B121" s="4"/>
-      <c r="C121" s="22"/>
-      <c r="D121" s="22"/>
-      <c r="E121" s="22"/>
-      <c r="F121" s="22"/>
-      <c r="G121" s="22"/>
-      <c r="H121" s="22"/>
       <c r="I121" s="5"/>
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B122" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C122" s="22"/>
-      <c r="D122" s="22"/>
-      <c r="E122" s="22"/>
-      <c r="F122" s="22"/>
-      <c r="G122" s="22"/>
-      <c r="H122" s="22"/>
       <c r="I122" s="5"/>
       <c r="J122" t="s">
         <v>24</v>
@@ -5906,12 +6830,6 @@
       <c r="B123" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C123" s="22"/>
-      <c r="D123" s="22"/>
-      <c r="E123" s="22"/>
-      <c r="F123" s="22"/>
-      <c r="G123" s="22"/>
-      <c r="H123" s="22"/>
       <c r="I123" s="5"/>
       <c r="J123" t="s">
         <v>24</v>
@@ -5924,12 +6842,6 @@
       <c r="B124" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C124" s="22"/>
-      <c r="D124" s="22"/>
-      <c r="E124" s="22"/>
-      <c r="F124" s="22"/>
-      <c r="G124" s="22"/>
-      <c r="H124" s="22"/>
       <c r="I124" s="5"/>
       <c r="K124" t="s">
         <v>127</v>
@@ -5946,7 +6858,7 @@
       <c r="I125" s="8"/>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A128" s="23" t="s">
+      <c r="A128" s="12" t="s">
         <v>128</v>
       </c>
       <c r="B128" s="2"/>
@@ -5971,376 +6883,70 @@
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A129" s="4"/>
-      <c r="B129" s="22"/>
-      <c r="C129" s="22"/>
-      <c r="D129" s="22"/>
-      <c r="E129" s="22"/>
-      <c r="F129" s="22"/>
-      <c r="G129" s="22"/>
-      <c r="H129" s="22"/>
-      <c r="I129" s="22"/>
-      <c r="J129" s="22"/>
-      <c r="K129" s="22"/>
-      <c r="L129" s="22"/>
-      <c r="M129" s="22"/>
-      <c r="N129" s="22"/>
-      <c r="O129" s="22"/>
-      <c r="P129" s="22"/>
-      <c r="Q129" s="22"/>
-      <c r="R129" s="22"/>
-      <c r="S129" s="22"/>
       <c r="T129" s="5"/>
     </row>
     <row r="130" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A130" s="4"/>
-      <c r="B130" s="22"/>
-      <c r="C130" s="22"/>
-      <c r="D130" s="22"/>
-      <c r="E130" s="22"/>
-      <c r="F130" s="22"/>
-      <c r="G130" s="22"/>
-      <c r="H130" s="22"/>
-      <c r="I130" s="22"/>
-      <c r="J130" s="22"/>
-      <c r="K130" s="22"/>
-      <c r="L130" s="22"/>
-      <c r="M130" s="22"/>
-      <c r="N130" s="22"/>
-      <c r="O130" s="22"/>
-      <c r="P130" s="22"/>
-      <c r="Q130" s="22"/>
-      <c r="R130" s="22"/>
-      <c r="S130" s="22"/>
       <c r="T130" s="5"/>
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A131" s="4"/>
-      <c r="B131" s="22"/>
-      <c r="C131" s="22"/>
-      <c r="D131" s="22"/>
-      <c r="E131" s="22"/>
-      <c r="F131" s="22"/>
-      <c r="G131" s="22"/>
-      <c r="H131" s="22"/>
-      <c r="I131" s="22"/>
-      <c r="J131" s="22"/>
-      <c r="K131" s="22"/>
-      <c r="L131" s="22"/>
-      <c r="M131" s="22"/>
-      <c r="N131" s="22"/>
-      <c r="O131" s="22"/>
-      <c r="P131" s="22"/>
-      <c r="Q131" s="22"/>
-      <c r="R131" s="22"/>
-      <c r="S131" s="22"/>
       <c r="T131" s="5"/>
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A132" s="4"/>
-      <c r="B132" s="22"/>
-      <c r="C132" s="22"/>
-      <c r="D132" s="22"/>
-      <c r="E132" s="22"/>
-      <c r="F132" s="22"/>
-      <c r="G132" s="22"/>
-      <c r="H132" s="22"/>
-      <c r="I132" s="22"/>
-      <c r="J132" s="22"/>
-      <c r="K132" s="22"/>
-      <c r="L132" s="22"/>
-      <c r="M132" s="22"/>
-      <c r="N132" s="22"/>
-      <c r="O132" s="22"/>
-      <c r="P132" s="22"/>
-      <c r="Q132" s="22"/>
-      <c r="R132" s="22"/>
-      <c r="S132" s="22"/>
       <c r="T132" s="5"/>
     </row>
     <row r="133" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A133" s="4"/>
-      <c r="B133" s="22"/>
-      <c r="C133" s="22"/>
-      <c r="D133" s="22"/>
-      <c r="E133" s="22"/>
-      <c r="F133" s="22"/>
-      <c r="G133" s="22"/>
-      <c r="H133" s="22"/>
-      <c r="I133" s="22"/>
-      <c r="J133" s="22"/>
-      <c r="K133" s="22"/>
-      <c r="L133" s="22"/>
-      <c r="M133" s="22"/>
-      <c r="N133" s="22"/>
-      <c r="O133" s="22"/>
-      <c r="P133" s="22"/>
-      <c r="Q133" s="22"/>
-      <c r="R133" s="22"/>
-      <c r="S133" s="22"/>
       <c r="T133" s="5"/>
     </row>
     <row r="134" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A134" s="4"/>
-      <c r="B134" s="22"/>
-      <c r="C134" s="22"/>
-      <c r="D134" s="22"/>
-      <c r="E134" s="22"/>
-      <c r="F134" s="22"/>
-      <c r="G134" s="22"/>
-      <c r="H134" s="22"/>
-      <c r="I134" s="22"/>
-      <c r="J134" s="22"/>
-      <c r="K134" s="22"/>
-      <c r="L134" s="22"/>
-      <c r="M134" s="22"/>
-      <c r="N134" s="22"/>
-      <c r="O134" s="22"/>
-      <c r="P134" s="22"/>
-      <c r="Q134" s="22"/>
-      <c r="R134" s="22"/>
-      <c r="S134" s="22"/>
       <c r="T134" s="5"/>
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A135" s="4"/>
-      <c r="B135" s="22"/>
-      <c r="C135" s="22"/>
-      <c r="D135" s="22"/>
-      <c r="E135" s="22"/>
-      <c r="F135" s="22"/>
-      <c r="G135" s="22"/>
-      <c r="H135" s="22"/>
-      <c r="I135" s="22"/>
-      <c r="J135" s="22"/>
-      <c r="K135" s="22"/>
-      <c r="L135" s="22"/>
-      <c r="M135" s="22"/>
-      <c r="N135" s="22"/>
-      <c r="O135" s="22"/>
-      <c r="P135" s="22"/>
-      <c r="Q135" s="22"/>
-      <c r="R135" s="22"/>
-      <c r="S135" s="22"/>
       <c r="T135" s="5"/>
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A136" s="4"/>
-      <c r="B136" s="22"/>
-      <c r="C136" s="22"/>
-      <c r="D136" s="22"/>
-      <c r="E136" s="22"/>
-      <c r="F136" s="22"/>
-      <c r="G136" s="22"/>
-      <c r="H136" s="22"/>
-      <c r="I136" s="22"/>
-      <c r="J136" s="22"/>
-      <c r="K136" s="22"/>
-      <c r="L136" s="22"/>
-      <c r="M136" s="22"/>
-      <c r="N136" s="22"/>
-      <c r="O136" s="22"/>
-      <c r="P136" s="22"/>
-      <c r="Q136" s="22"/>
-      <c r="R136" s="22"/>
-      <c r="S136" s="22"/>
       <c r="T136" s="5"/>
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A137" s="4"/>
-      <c r="B137" s="22"/>
-      <c r="C137" s="22"/>
-      <c r="D137" s="22"/>
-      <c r="E137" s="22"/>
-      <c r="F137" s="22"/>
-      <c r="G137" s="22"/>
-      <c r="H137" s="22"/>
-      <c r="I137" s="22"/>
-      <c r="J137" s="22"/>
-      <c r="K137" s="22"/>
-      <c r="L137" s="22"/>
-      <c r="M137" s="22"/>
-      <c r="N137" s="22"/>
-      <c r="O137" s="22"/>
-      <c r="P137" s="22"/>
-      <c r="Q137" s="22"/>
-      <c r="R137" s="22"/>
-      <c r="S137" s="22"/>
       <c r="T137" s="5"/>
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A138" s="4"/>
-      <c r="B138" s="22"/>
-      <c r="C138" s="22"/>
-      <c r="D138" s="22"/>
-      <c r="E138" s="22"/>
-      <c r="F138" s="22"/>
-      <c r="G138" s="22"/>
-      <c r="H138" s="22"/>
-      <c r="I138" s="22"/>
-      <c r="J138" s="22"/>
-      <c r="K138" s="22"/>
-      <c r="L138" s="22"/>
-      <c r="M138" s="22"/>
-      <c r="N138" s="22"/>
-      <c r="O138" s="22"/>
-      <c r="P138" s="22"/>
-      <c r="Q138" s="22"/>
-      <c r="R138" s="22"/>
-      <c r="S138" s="22"/>
       <c r="T138" s="5"/>
     </row>
     <row r="139" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A139" s="4"/>
-      <c r="B139" s="22"/>
-      <c r="C139" s="22"/>
-      <c r="D139" s="22"/>
-      <c r="E139" s="22"/>
-      <c r="F139" s="22"/>
-      <c r="G139" s="22"/>
-      <c r="H139" s="22"/>
-      <c r="I139" s="22"/>
-      <c r="J139" s="22"/>
-      <c r="K139" s="22"/>
-      <c r="L139" s="22"/>
-      <c r="M139" s="22"/>
-      <c r="N139" s="22"/>
-      <c r="O139" s="22"/>
-      <c r="P139" s="22"/>
-      <c r="Q139" s="22"/>
-      <c r="R139" s="22"/>
-      <c r="S139" s="22"/>
       <c r="T139" s="5"/>
     </row>
     <row r="140" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A140" s="4"/>
-      <c r="B140" s="22"/>
-      <c r="C140" s="22"/>
-      <c r="D140" s="22"/>
-      <c r="E140" s="22"/>
-      <c r="F140" s="22"/>
-      <c r="G140" s="22"/>
-      <c r="H140" s="22"/>
-      <c r="I140" s="22"/>
-      <c r="J140" s="22"/>
-      <c r="K140" s="22"/>
-      <c r="L140" s="22"/>
-      <c r="M140" s="22"/>
-      <c r="N140" s="22"/>
-      <c r="O140" s="22"/>
-      <c r="P140" s="22"/>
-      <c r="Q140" s="22"/>
-      <c r="R140" s="22"/>
-      <c r="S140" s="22"/>
       <c r="T140" s="5"/>
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A141" s="4"/>
-      <c r="B141" s="22"/>
-      <c r="C141" s="22"/>
-      <c r="D141" s="22"/>
-      <c r="E141" s="22"/>
-      <c r="F141" s="22"/>
-      <c r="G141" s="22"/>
-      <c r="H141" s="22"/>
-      <c r="I141" s="22"/>
-      <c r="J141" s="22"/>
-      <c r="K141" s="22"/>
-      <c r="L141" s="22"/>
-      <c r="M141" s="22"/>
-      <c r="N141" s="22"/>
-      <c r="O141" s="22"/>
-      <c r="P141" s="22"/>
-      <c r="Q141" s="22"/>
-      <c r="R141" s="22"/>
-      <c r="S141" s="22"/>
       <c r="T141" s="5"/>
     </row>
     <row r="142" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A142" s="4"/>
-      <c r="B142" s="22"/>
-      <c r="C142" s="22"/>
-      <c r="D142" s="22"/>
-      <c r="E142" s="22"/>
-      <c r="F142" s="22"/>
-      <c r="G142" s="22"/>
-      <c r="H142" s="22"/>
-      <c r="I142" s="22"/>
-      <c r="J142" s="22"/>
-      <c r="K142" s="22"/>
-      <c r="L142" s="22"/>
-      <c r="M142" s="22"/>
-      <c r="N142" s="22"/>
-      <c r="O142" s="22"/>
-      <c r="P142" s="22"/>
-      <c r="Q142" s="22"/>
-      <c r="R142" s="22"/>
-      <c r="S142" s="22"/>
       <c r="T142" s="5"/>
     </row>
     <row r="143" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A143" s="4"/>
-      <c r="B143" s="22"/>
-      <c r="C143" s="22"/>
-      <c r="D143" s="22"/>
-      <c r="E143" s="22"/>
-      <c r="F143" s="22"/>
-      <c r="G143" s="22"/>
-      <c r="H143" s="22"/>
-      <c r="I143" s="22"/>
-      <c r="J143" s="22"/>
-      <c r="K143" s="22"/>
-      <c r="L143" s="22"/>
-      <c r="M143" s="22"/>
-      <c r="N143" s="22"/>
-      <c r="O143" s="22"/>
-      <c r="P143" s="22"/>
-      <c r="Q143" s="22"/>
-      <c r="R143" s="22"/>
-      <c r="S143" s="22"/>
       <c r="T143" s="5"/>
     </row>
     <row r="144" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A144" s="4"/>
-      <c r="B144" s="22"/>
-      <c r="C144" s="22"/>
-      <c r="D144" s="22"/>
-      <c r="E144" s="22"/>
-      <c r="F144" s="22"/>
-      <c r="G144" s="22"/>
-      <c r="H144" s="22"/>
-      <c r="I144" s="22"/>
-      <c r="J144" s="22"/>
-      <c r="K144" s="22"/>
-      <c r="L144" s="22"/>
-      <c r="M144" s="22"/>
-      <c r="N144" s="22"/>
-      <c r="O144" s="22"/>
-      <c r="P144" s="22"/>
-      <c r="Q144" s="22"/>
-      <c r="R144" s="22"/>
-      <c r="S144" s="22"/>
       <c r="T144" s="5"/>
     </row>
     <row r="145" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A145" s="4"/>
-      <c r="B145" s="22"/>
-      <c r="C145" s="22"/>
-      <c r="D145" s="22"/>
-      <c r="E145" s="22"/>
-      <c r="F145" s="22"/>
-      <c r="G145" s="22"/>
-      <c r="H145" s="22"/>
-      <c r="I145" s="22"/>
-      <c r="J145" s="22"/>
-      <c r="K145" s="22"/>
-      <c r="L145" s="22"/>
-      <c r="M145" s="22"/>
-      <c r="N145" s="22"/>
-      <c r="O145" s="22"/>
-      <c r="P145" s="22"/>
-      <c r="Q145" s="22"/>
-      <c r="R145" s="22"/>
-      <c r="S145" s="22"/>
       <c r="T145" s="5"/>
     </row>
     <row r="146" spans="1:20" x14ac:dyDescent="0.2">
@@ -6372,4 +6978,832 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68644A1-6143-3D43-8EE4-0A04A124DB26}">
+  <dimension ref="A3:K190"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V182" sqref="V182"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="4"/>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="4"/>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="E29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="4"/>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="4"/>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="C32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="4"/>
+      <c r="D33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="4"/>
+      <c r="E34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="4"/>
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="4"/>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="4"/>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="4"/>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="4"/>
+      <c r="D39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" s="4"/>
+      <c r="E40" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B41" s="4"/>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B42" s="4"/>
+      <c r="D42" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" s="9"/>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B43" s="4"/>
+      <c r="E43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="4"/>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="4"/>
+      <c r="E45" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="4"/>
+      <c r="E46" t="s">
+        <v>49</v>
+      </c>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="4"/>
+      <c r="E47" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B48" s="6"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B53" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B54" s="4"/>
+      <c r="C54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B55" s="4"/>
+      <c r="D55" t="s">
+        <v>31</v>
+      </c>
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B56" s="4"/>
+      <c r="D56" t="s">
+        <v>32</v>
+      </c>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B57" s="4"/>
+      <c r="D57" t="s">
+        <v>33</v>
+      </c>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B58" s="4"/>
+      <c r="C58" t="s">
+        <v>34</v>
+      </c>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B59" s="4"/>
+      <c r="C59" t="s">
+        <v>35</v>
+      </c>
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B60" s="4"/>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B61" s="4"/>
+      <c r="C61" t="s">
+        <v>36</v>
+      </c>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B62" s="4"/>
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B63" s="4"/>
+      <c r="C63" t="s">
+        <v>37</v>
+      </c>
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B64" s="4"/>
+      <c r="D64" t="s">
+        <v>38</v>
+      </c>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B65" s="4"/>
+      <c r="C65" t="s">
+        <v>39</v>
+      </c>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B66" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B67" s="4"/>
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B68" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B69" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B70" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B71" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B72" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B73" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B74" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B75" s="4"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B76" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B77" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B78" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B79" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B80" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B81" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B82" s="4"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B83" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B84" s="4"/>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B85" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B86" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B87" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B88" s="4"/>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B89" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B90" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="I90" s="5"/>
+      <c r="J90" t="s">
+        <v>24</v>
+      </c>
+      <c r="K90" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B91" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="I91" s="5"/>
+      <c r="K91" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B92" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="I92" s="5"/>
+      <c r="J92" t="s">
+        <v>24</v>
+      </c>
+      <c r="K92" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B93" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B94" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B95" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I95" s="5"/>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B96" s="4"/>
+      <c r="I96" s="5"/>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B97" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I97" s="5"/>
+      <c r="J97" t="s">
+        <v>24</v>
+      </c>
+      <c r="K97" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B98" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="I98" s="5"/>
+      <c r="J98" t="s">
+        <v>24</v>
+      </c>
+      <c r="K98" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B99" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="I99" s="5"/>
+      <c r="J99" t="s">
+        <v>24</v>
+      </c>
+      <c r="K99" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B100" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="I100" s="5"/>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B101" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="I101" s="5"/>
+      <c r="J101" t="s">
+        <v>24</v>
+      </c>
+      <c r="K101" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B102" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I102" s="5"/>
+      <c r="K102" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B103" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I103" s="5"/>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B104" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I104" s="5"/>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B105" s="4"/>
+      <c r="I105" s="5"/>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B106" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I106" s="5"/>
+    </row>
+    <row r="107" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B107" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="I107" s="5"/>
+    </row>
+    <row r="108" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B108" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I108" s="5"/>
+    </row>
+    <row r="109" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B109" s="4"/>
+      <c r="I109" s="5"/>
+    </row>
+    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B110" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="I110" s="5"/>
+      <c r="J110" t="s">
+        <v>24</v>
+      </c>
+      <c r="K110" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B111" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I111" s="5"/>
+    </row>
+    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B112" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="I112" s="5"/>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B113" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I113" s="5"/>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B114" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="I114" s="5"/>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B115" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="I115" s="5"/>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B116" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="I116" s="5"/>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B117" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I117" s="5"/>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B118" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I118" s="5"/>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B119" s="6"/>
+      <c r="C119" s="7"/>
+      <c r="D119" s="7"/>
+      <c r="E119" s="7"/>
+      <c r="F119" s="7"/>
+      <c r="G119" s="7"/>
+      <c r="H119" s="7"/>
+      <c r="I119" s="8"/>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B163" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B164" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B190" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>